<commit_message>
Some new scenes with raycast
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Tasklist</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Model Collision recognition in Unity</t>
+  </si>
+  <si>
+    <t>Install Vive at home</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +648,9 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Scene 1 began, with room modelled and new assets
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Tasklist</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Install Vive at home</t>
+  </si>
+  <si>
+    <t>Find early assets to build with</t>
   </si>
 </sst>
 </file>
@@ -537,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,8 +584,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
+      <c r="A3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -599,7 +602,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>22</v>
@@ -613,7 +616,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -623,33 +626,40 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Physics materials and custom grip function
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -543,7 +543,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,16 +618,16 @@
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>14</v>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Finished rotating/centrifuge first example. started steamtrain with coal spawner and trigger
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Tasklist</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Find early assets to build with</t>
+  </si>
+  <si>
+    <t>Add Centrifugal Forces</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +661,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Added custom interaction events.
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -238,11 +238,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -560,28 +560,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" t="s">
         <v>1</v>
       </c>
@@ -652,10 +652,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -666,9 +663,6 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -702,6 +696,16 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>